<commit_message>
feat : rewardTable 작업중
</commit_message>
<xml_diff>
--- a/URPRagProjectSingle/Assets/Characters/Skills/DataSheet/QuestDetailSheet.xlsx
+++ b/URPRagProjectSingle/Assets/Characters/Skills/DataSheet/QuestDetailSheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>questID</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>로라스의 요구대로 슬라임들을 처치했습니다. 로라스에게 보고하십시오</t>
+  </si>
+  <si>
+    <t>M_Slime</t>
+  </si>
+  <si>
+    <t>MOB_Slime</t>
   </si>
 </sst>
 </file>
@@ -443,13 +449,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -464,7 +469,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -473,7 +477,6 @@
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -482,7 +485,6 @@
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -491,7 +493,6 @@
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -506,7 +507,6 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -521,7 +521,6 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -536,7 +535,6 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -545,7 +543,6 @@
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -556,13 +553,6 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -714,20 +704,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1051,7 +1029,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1087,7 +1065,7 @@
       <c r="A2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1104,7 +1082,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="0" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -1124,14 +1102,14 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D4" s="0">
         <v>1</v>
@@ -1144,7 +1122,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="0" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="0" t="s">

</xml_diff>